<commit_message>
projeto finalizado com sucesso
</commit_message>
<xml_diff>
--- a/HistoricoVersoes (5).xlsx
+++ b/HistoricoVersoes (5).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://embraer-my.sharepoint.com/personal/denis_fermino_embraer_com_br/Documents/version history/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSOUZA14\Music\PANDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="11_0852B79F14480E8F6C5130B652245E3FE408A75F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7E3F32E-E4A2-4C99-AD92-14160D308A9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA40DC98-1277-4376-B1AB-DBF49E2A5F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -148,6 +148,60 @@
   </si>
   <si>
     <t>2025-09-16T16:27:15Z</t>
+  </si>
+  <si>
+    <t>particulado</t>
+  </si>
+  <si>
+    <t>2025-09-15T23:15:01Z</t>
+  </si>
+  <si>
+    <t>ESCORRIDO</t>
+  </si>
+  <si>
+    <t>2025-09-15T23:54:45Z</t>
+  </si>
+  <si>
+    <t>vazado de tinta</t>
+  </si>
+  <si>
+    <t>2025-09-16T00:32:53Z</t>
+  </si>
+  <si>
+    <t>2025-09-16T00:34:45Z</t>
+  </si>
+  <si>
+    <t>desplacado</t>
+  </si>
+  <si>
+    <t>2025-09-16T00:35:50Z</t>
+  </si>
+  <si>
+    <t>desplacado na asa</t>
+  </si>
+  <si>
+    <t>2025-09-16T00:39:02Z</t>
+  </si>
+  <si>
+    <t>vazado no selo</t>
+  </si>
+  <si>
+    <t>Particulado</t>
+  </si>
+  <si>
+    <t>teste teste</t>
+  </si>
+  <si>
+    <t>2025-09-15T23:21:25Z</t>
+  </si>
+  <si>
+    <t>ESCORRIDO NA CARENAGEM</t>
+  </si>
+  <si>
+    <t>desplacado no bordo</t>
+  </si>
+  <si>
+    <t>teste</t>
   </si>
 </sst>
 </file>
@@ -207,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -218,18 +272,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,13 +393,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
-<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3374AD9-82CA-4148-A0CF-834D4F35DDE2}" name="historicodeversões" displayName="historicodeversões" ref="A1:H47" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A1:H47" xr:uid="{F3374AD9-82CA-4148-A0CF-834D4F35DDE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3374AD9-82CA-4148-A0CF-834D4F35DDE2}" name="historicodeversões" displayName="historicodeversões" ref="A1:H102" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:H102" xr:uid="{F3374AD9-82CA-4148-A0CF-834D4F35DDE2}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C7D95DEC-2D4B-4F64-BA59-830286B0E7EB}" name="ID"/>
     <tableColumn id="6" xr3:uid="{577A0115-A26B-48D2-A881-6EA50665DBE5}" name="Praetor" dataDxfId="3"/>
@@ -669,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,38 +756,38 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>19</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="2">
         <v>20250</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -769,7 +811,7 @@
       <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -779,7 +821,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -789,7 +831,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -813,7 +855,7 @@
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -823,7 +865,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
@@ -833,7 +875,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
@@ -843,7 +885,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -867,7 +909,7 @@
       <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
@@ -877,7 +919,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -887,7 +929,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -897,7 +939,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -907,7 +949,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -931,7 +973,7 @@
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
@@ -941,7 +983,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
@@ -951,7 +993,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -961,7 +1003,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
@@ -971,7 +1013,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -981,7 +1023,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -1005,7 +1047,7 @@
       <c r="G22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
@@ -1015,7 +1057,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="4"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
@@ -1025,7 +1067,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
@@ -1035,7 +1077,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
@@ -1045,7 +1087,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="4"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
@@ -1055,7 +1097,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
@@ -1065,7 +1107,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
@@ -1075,7 +1117,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
@@ -1085,7 +1127,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
@@ -1109,7 +1151,7 @@
       <c r="G31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
@@ -1119,7 +1161,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
@@ -1143,7 +1185,7 @@
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="4"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
@@ -1153,7 +1195,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="4"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
@@ -1163,7 +1205,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
@@ -1173,7 +1215,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="4"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
@@ -1183,7 +1225,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="4"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -1207,7 +1249,7 @@
       <c r="G38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H38" s="4"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
@@ -1217,7 +1259,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="4"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
@@ -1227,7 +1269,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="4"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
@@ -1237,7 +1279,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="4"/>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
@@ -1261,62 +1303,999 @@
       <c r="G42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H42" s="4"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="2">
+        <v>6</v>
+      </c>
+      <c r="B43" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="4"/>
+      <c r="F43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="2">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="4"/>
+      <c r="F44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="2">
+        <v>6</v>
+      </c>
+      <c r="B45" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="4"/>
+      <c r="F45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="2">
+        <v>8</v>
+      </c>
+      <c r="B46" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="4"/>
+      <c r="E46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="2">
+        <v>9</v>
+      </c>
+      <c r="B47" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="4"/>
+      <c r="E47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>10</v>
+      </c>
+      <c r="B48" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>11</v>
+      </c>
+      <c r="B49" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>12</v>
+      </c>
+      <c r="B50" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>10</v>
+      </c>
+      <c r="B51" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>7</v>
+      </c>
+      <c r="B52" s="2">
+        <v>10156</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>12</v>
+      </c>
+      <c r="B53" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>8</v>
+      </c>
+      <c r="B54" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>11</v>
+      </c>
+      <c r="B55" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>7</v>
+      </c>
+      <c r="B57" s="2">
+        <v>10156</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>12</v>
+      </c>
+      <c r="B58" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>11</v>
+      </c>
+      <c r="B59" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>10</v>
+      </c>
+      <c r="B60" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>9</v>
+      </c>
+      <c r="B61" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>8</v>
+      </c>
+      <c r="B62" s="2">
+        <v>20242</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>19</v>
+      </c>
+      <c r="B63" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>19</v>
+      </c>
+      <c r="B65" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>19</v>
+      </c>
+      <c r="B72" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>19</v>
+      </c>
+      <c r="B83" s="2">
+        <v>20250</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>20</v>
+      </c>
+      <c r="B92" s="2">
+        <v>20259</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>20</v>
+      </c>
+      <c r="B94" s="2">
+        <v>20259</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>20</v>
+      </c>
+      <c r="B99" s="2">
+        <v>20259</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>